<commit_message>
Izmena imena u excell fajlu
</commit_message>
<xml_diff>
--- a/zavrsniProjekat/data.xlsx
+++ b/zavrsniProjekat/data.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24131"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB5DCC91-BF80-427E-B14E-B480CF43BC2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,9 +35,6 @@
     <t>zika@gmail.com</t>
   </si>
   <si>
-    <t>Branka</t>
-  </si>
-  <si>
     <t>Ilic</t>
   </si>
   <si>
@@ -59,12 +57,15 @@
   </si>
   <si>
     <t>ana@gmail.com</t>
+  </si>
+  <si>
+    <t>Branko</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -200,6 +201,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -235,6 +253,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -410,11 +445,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -447,44 +482,44 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C1" r:id="rId1"/>
-    <hyperlink ref="C2" r:id="rId2"/>
-    <hyperlink ref="C3" r:id="rId3"/>
-    <hyperlink ref="C4" r:id="rId4"/>
-    <hyperlink ref="C5" r:id="rId5"/>
+    <hyperlink ref="C1" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C3" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="C4" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="C5" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>